<commit_message>
Modified Report and Test Cases
</commit_message>
<xml_diff>
--- a/nopCommerceV2/src/test/java/com/nopcommerce/testData/LoginData.xlsx
+++ b/nopCommerceV2/src/test/java/com/nopcommerce/testData/LoginData.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB22E21-11C8-443D-B149-57AE29D8B199}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFEF460-7C71-4F3A-990B-96B1BFC32B63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>username</t>
   </si>
@@ -38,6 +39,63 @@
   </si>
   <si>
     <t>adm@yourstore.com</t>
+  </si>
+  <si>
+    <t>pwd1</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>CustomerRoles</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>ManagerOfVendor</t>
+  </si>
+  <si>
+    <t>Vendor 2</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Jagadeesh</t>
+  </si>
+  <si>
+    <t>Patil</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>busyQA</t>
+  </si>
+  <si>
+    <t>AdminContent</t>
+  </si>
+  <si>
+    <t>This is for testing.........</t>
+  </si>
+  <si>
+    <t>The new customer has been added successfully</t>
+  </si>
+  <si>
+    <t>Exmessage</t>
   </si>
 </sst>
 </file>
@@ -118,11 +176,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,17 +502,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -466,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -474,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -482,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -500,4 +562,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBE1CF4-61FD-43B8-A0A9-A5177DB13BAE}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="6">
+        <v>31233</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{028514F6-0EA5-456C-AC29-48C21F376032}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>